<commit_message>
menambahkan kolom warna dan kondisi pada produk handphone
</commit_message>
<xml_diff>
--- a/storage/app/public/assets/format_handphone.xlsx
+++ b/storage/app/public/assets/format_handphone.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\servis-online\public\storage\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khaed\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D575F766-63F8-4036-86AC-E7788590F85A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D0F3BB-5BFE-45F1-B501-3D942FDF65A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Nama Produk</t>
   </si>
@@ -65,6 +65,18 @@
   </si>
   <si>
     <t>ID Kapasitas</t>
+  </si>
+  <si>
+    <t>Warna</t>
+  </si>
+  <si>
+    <t>Kondisi</t>
+  </si>
+  <si>
+    <t>NEW</t>
+  </si>
+  <si>
+    <t>SECOND</t>
   </si>
 </sst>
 </file>
@@ -432,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A1:XFD1048576"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -444,19 +456,19 @@
     <col min="2" max="2" width="11.5546875" customWidth="1"/>
     <col min="3" max="3" width="13.33203125" customWidth="1"/>
     <col min="4" max="4" width="11.44140625" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.6640625" customWidth="1"/>
-    <col min="8" max="8" width="9.5546875" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" customWidth="1"/>
-    <col min="10" max="10" width="14.33203125" customWidth="1"/>
-    <col min="11" max="11" width="16.33203125" customWidth="1"/>
-    <col min="12" max="12" width="19.44140625" customWidth="1"/>
-    <col min="13" max="13" width="18.88671875" customWidth="1"/>
-    <col min="14" max="14" width="16.44140625" customWidth="1"/>
+    <col min="5" max="7" width="13.5546875" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.6640625" customWidth="1"/>
+    <col min="10" max="10" width="9.5546875" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" customWidth="1"/>
+    <col min="12" max="12" width="14.33203125" customWidth="1"/>
+    <col min="13" max="13" width="16.33203125" customWidth="1"/>
+    <col min="14" max="14" width="19.44140625" customWidth="1"/>
+    <col min="15" max="15" width="18.88671875" customWidth="1"/>
+    <col min="16" max="16" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -472,35 +484,51 @@
       <c r="E1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="G3" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add kolom tgl masuk
</commit_message>
<xml_diff>
--- a/storage/app/public/assets/format_handphone.xlsx
+++ b/storage/app/public/assets/format_handphone.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khaed\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\servis-online\public\storage\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D0F3BB-5BFE-45F1-B501-3D942FDF65A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{287AD7FF-E798-4C36-8721-1FDF76D91D88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Nama Produk</t>
   </si>
@@ -76,7 +76,13 @@
     <t>NEW</t>
   </si>
   <si>
+    <t>Tgl Masuk</t>
+  </si>
+  <si>
     <t>SECOND</t>
+  </si>
+  <si>
+    <t>2023-12-30 00:00:00</t>
   </si>
 </sst>
 </file>
@@ -135,11 +141,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -466,9 +473,10 @@
     <col min="14" max="14" width="19.44140625" customWidth="1"/>
     <col min="15" max="15" width="18.88671875" customWidth="1"/>
     <col min="16" max="16" width="16.44140625" customWidth="1"/>
+    <col min="18" max="18" width="19.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -520,15 +528,41 @@
       <c r="Q1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="R1" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="G2" t="s">
         <v>17</v>
       </c>
+      <c r="O2">
+        <v>365</v>
+      </c>
+      <c r="P2">
+        <v>365</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="G3" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="O3">
+        <v>30</v>
+      </c>
+      <c r="P3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="O4">
+        <v>7</v>
+      </c>
+      <c r="P4">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>